<commit_message>
Change logic program and fix problem of color
</commit_message>
<xml_diff>
--- a/excelFiles/text.xlsx
+++ b/excelFiles/text.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,7 +27,13 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color rgb="FFFFFFFF"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -40,12 +46,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF4CAF50"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4CAF50"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -80,18 +86,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,140 +480,133 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Список зарегистрированных пользователей</t>
+          <t>Имя</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Фамилия</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Возраст</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Город</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Дата регистрации</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Имя</t>
+          <t>Иван</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Фамилия</t>
+          <t>Иванов</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Возраст</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Город</t>
+          <t>Москва</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Дата регистрации</t>
+          <t>2025-06-25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Иван</t>
+          <t>Анна</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>Иванов</t>
+          <t>Петрова</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>31</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2025-06-25</t>
+          <t>2024-12-13</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Анна</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Петрова</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Санкт-Петербург</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>2024-12-13</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Олег</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Сидоров</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Новосибирск</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>2023-05-03</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Олег</t>
+          <t>Елена</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Сидоров</t>
+          <t>Морозова</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>2023-05-03</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Елена</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Морозова</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Казань</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
         <is>
           <t>2025-01-15</t>
         </is>

</xml_diff>